<commit_message>
Updated BOMs for alternate part so that it doesn't need backordered from LCSC
</commit_message>
<xml_diff>
--- a/LCSC_Bom.xlsx
+++ b/LCSC_Bom.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4587D786-8055-4749-9B47-34E876782651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20383514-CAC8-4505-86FF-9075B043AB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2910" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BomTmpl" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Quantity</t>
   </si>
@@ -41,13 +51,190 @@
   </si>
   <si>
     <t>Customer Part Number(optional)</t>
+  </si>
+  <si>
+    <t>CL10C200JB8NNNC</t>
+  </si>
+  <si>
+    <t>CL10C100JB8NNNC</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>CA45-A-16V-1uF-K</t>
+  </si>
+  <si>
+    <t>CL10A335KP8NNNC</t>
+  </si>
+  <si>
+    <t>TAJA106K016RNJ</t>
+  </si>
+  <si>
+    <t>CL10A105KB8NNNC</t>
+  </si>
+  <si>
+    <t>1N4148W</t>
+  </si>
+  <si>
+    <t>MC-311D</t>
+  </si>
+  <si>
+    <t>0603WAF200JT5E</t>
+  </si>
+  <si>
+    <t>0603WAF1002T5E</t>
+  </si>
+  <si>
+    <t>0603WAF5101T5E</t>
+  </si>
+  <si>
+    <t>0603WAF1501T5E</t>
+  </si>
+  <si>
+    <t>0603WAF1001T5E</t>
+  </si>
+  <si>
+    <t>TS-1187A-C-C-B</t>
+  </si>
+  <si>
+    <t>EC11E1534408</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>MTF185-104SY1</t>
+  </si>
+  <si>
+    <t>X50328MSB4SI</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>Shenzhen Zhenhua XinYun Elec</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>Semtech</t>
+  </si>
+  <si>
+    <t>SOFNG</t>
+  </si>
+  <si>
+    <t>Uniroyal Elec</t>
+  </si>
+  <si>
+    <t>XKB Enterprise</t>
+  </si>
+  <si>
+    <t>ALPS Electric</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>MINTRON</t>
+  </si>
+  <si>
+    <t>Yangxing Tech</t>
+  </si>
+  <si>
+    <t>Seiko Epson</t>
+  </si>
+  <si>
+    <t>C1648</t>
+  </si>
+  <si>
+    <t>C1634</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>C140386</t>
+  </si>
+  <si>
+    <t>C51412</t>
+  </si>
+  <si>
+    <t>C7171</t>
+  </si>
+  <si>
+    <t>C15849</t>
+  </si>
+  <si>
+    <t>C81598</t>
+  </si>
+  <si>
+    <t>C136423</t>
+  </si>
+  <si>
+    <t>C22950</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C23186</t>
+  </si>
+  <si>
+    <t>C22843</t>
+  </si>
+  <si>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>C318889</t>
+  </si>
+  <si>
+    <t>C278348</t>
+  </si>
+  <si>
+    <t>C8734</t>
+  </si>
+  <si>
+    <t>C7519</t>
+  </si>
+  <si>
+    <t>C358718</t>
+  </si>
+  <si>
+    <t>C157341</t>
+  </si>
+  <si>
+    <t>UMW(Youtai Semiconductor Co., Ltd.)</t>
+  </si>
+  <si>
+    <t>C347222</t>
+  </si>
+  <si>
+    <t>X1A000141000100</t>
+  </si>
+  <si>
+    <t>C94674</t>
+  </si>
+  <si>
+    <t>Ext Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -58,13 +245,44 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF525252"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF525252"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,9 +297,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,47 +620,449 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>(A2*5)+_xlfn.CEILING.MATH(0.4*(A2*5))</f>
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B23" si="0">(A3*5)+_xlfn.CEILING.MATH(0.4*(A3*5))</f>
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOMs to reflect changes
</commit_message>
<xml_diff>
--- a/LCSC_Bom.xlsx
+++ b/LCSC_Bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20383514-CAC8-4505-86FF-9075B043AB72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABAC9D3-A5F1-4A02-B582-1699CC4E1D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2910" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BomTmpl" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Quantity</t>
   </si>
@@ -116,6 +116,9 @@
     <t>X50328MSB4SI</t>
   </si>
   <si>
+    <t>Q13FC1350000200</t>
+  </si>
+  <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
@@ -146,6 +149,9 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
+    <t>Advanced Monolithic Systems</t>
+  </si>
+  <si>
     <t>MINTRON</t>
   </si>
   <si>
@@ -206,6 +212,9 @@
     <t>C8734</t>
   </si>
   <si>
+    <t>C6186</t>
+  </si>
+  <si>
     <t>C7519</t>
   </si>
   <si>
@@ -215,19 +224,25 @@
     <t>C157341</t>
   </si>
   <si>
-    <t>UMW(Youtai Semiconductor Co., Ltd.)</t>
-  </si>
-  <si>
-    <t>C347222</t>
-  </si>
-  <si>
-    <t>X1A000141000100</t>
-  </si>
-  <si>
-    <t>C94674</t>
+    <t>C48615</t>
   </si>
   <si>
     <t>Ext Quantity</t>
+  </si>
+  <si>
+    <t>CL10A106MA8NRNC</t>
+  </si>
+  <si>
+    <t>C96446</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>KEXIN</t>
+  </si>
+  <si>
+    <t>C489349</t>
   </si>
 </sst>
 </file>
@@ -620,10 +635,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,43 +683,43 @@
       <c r="A2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <f>(A2*5)+_xlfn.CEILING.MATH(0.4*(A2*5))</f>
+      <c r="B2">
+        <f>(A2*5)+(0.4*(A2*5))</f>
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ref="B3:B23" si="0">(A3*5)+_xlfn.CEILING.MATH(0.4*(A3*5))</f>
+      <c r="B3">
+        <f t="shared" ref="B3:B25" si="0">(A3*5)+(0.4*(A3*5))</f>
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>27</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>189</v>
       </c>
@@ -712,17 +727,17 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -730,17 +745,17 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -748,17 +763,17 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -766,17 +781,17 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -784,97 +799,97 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2">
-        <f t="shared" si="0"/>
-        <v>133</v>
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>52</v>
@@ -882,17 +897,17 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>91</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>53</v>
@@ -900,17 +915,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>54</v>
@@ -920,12 +935,12 @@
       <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>35</v>
@@ -936,17 +951,17 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>56</v>
@@ -956,15 +971,15 @@
       <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>57</v>
@@ -972,91 +987,127 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>59</v>
+        <v>24</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BOMs (to fix some duplicate items issues) and added a cost spreadsheet to keep up with the cost of the prototype design
</commit_message>
<xml_diff>
--- a/LCSC_Bom.xlsx
+++ b/LCSC_Bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABAC9D3-A5F1-4A02-B582-1699CC4E1D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9B0AAD-CC08-467D-BEAE-229C8C17C3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2910" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>X50328MSB4SI</t>
   </si>
   <si>
-    <t>Q13FC1350000200</t>
-  </si>
-  <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>Advanced Monolithic Systems</t>
-  </si>
-  <si>
     <t>MINTRON</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>C8734</t>
   </si>
   <si>
-    <t>C6186</t>
-  </si>
-  <si>
     <t>C7519</t>
   </si>
   <si>
@@ -224,9 +215,6 @@
     <t>C157341</t>
   </si>
   <si>
-    <t>C48615</t>
-  </si>
-  <si>
     <t>Ext Quantity</t>
   </si>
   <si>
@@ -243,6 +231,18 @@
   </si>
   <si>
     <t>C489349</t>
+  </si>
+  <si>
+    <t>C347222</t>
+  </si>
+  <si>
+    <t>UMW(Youtai Semiconductor Co., Ltd.)</t>
+  </si>
+  <si>
+    <t>C94674</t>
+  </si>
+  <si>
+    <t>X1A000141000100</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +646,7 @@
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -691,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -709,10 +709,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -727,10 +727,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -745,10 +745,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.35">
@@ -763,10 +763,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -781,10 +781,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -799,10 +799,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -814,13 +814,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -835,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -853,10 +853,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -868,13 +868,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -889,10 +889,10 @@
         <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,10 +907,10 @@
         <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -925,10 +925,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -943,10 +943,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,10 +961,10 @@
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -979,10 +979,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,10 +997,10 @@
         <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1015,10 +1015,10 @@
         <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1033,10 +1033,10 @@
         <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1051,10 +1051,10 @@
         <v>25</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1069,10 +1069,10 @@
         <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1087,10 +1087,10 @@
         <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1102,13 +1102,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated boms with another alternate part, 0.1uf resistors were OOS
</commit_message>
<xml_diff>
--- a/LCSC_Bom.xlsx
+++ b/LCSC_Bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9B0AAD-CC08-467D-BEAE-229C8C17C3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A8533-23DE-4EDE-A09C-6F5BE74B9DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2910" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BomTmpl" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>CL10C100JB8NNNC</t>
   </si>
   <si>
-    <t>CC0603KRX7R9BB104</t>
-  </si>
-  <si>
     <t>CA45-A-16V-1uF-K</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>Shenzhen Zhenhua XinYun Elec</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>C1634</t>
   </si>
   <si>
-    <t>C14663</t>
-  </si>
-  <si>
     <t>C140386</t>
   </si>
   <si>
@@ -243,6 +234,15 @@
   </si>
   <si>
     <t>X1A000141000100</t>
+  </si>
+  <si>
+    <t>FN18F104Z500PSG</t>
+  </si>
+  <si>
+    <t>PSA(Prosperity Dielectrics)</t>
+  </si>
+  <si>
+    <t>C497032</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -691,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -709,10 +709,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -724,13 +724,13 @@
         <v>189</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -742,13 +742,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.35">
@@ -760,13 +760,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -778,13 +778,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -796,13 +796,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -814,13 +814,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -832,13 +832,13 @@
         <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -850,13 +850,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -868,13 +868,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -886,31 +886,31 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -922,13 +922,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -940,13 +940,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -958,13 +958,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -976,13 +976,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -994,13 +994,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1012,13 +1012,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,13 +1030,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1048,13 +1048,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1066,13 +1066,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1084,13 +1084,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1102,13 +1102,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>